<commit_message>
local photoelectric double graph ver.5
</commit_message>
<xml_diff>
--- a/Photoelectric/계산식.xlsx
+++ b/Photoelectric/계산식.xlsx
@@ -3,7 +3,7 @@
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:fileVersion appName="HCell" lastEdited="9.1" lowestEdited="9.1" rupBuild="1.3237"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="28395" windowHeight="12210" tabRatio="500"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="28365" windowHeight="8280" tabRatio="500"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -17,73 +17,115 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <x:si>
+    <x:t>Cs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>K</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Na</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Li</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m(electrons' mass)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c(light velocity)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>velocity_real</x:t>
+  </x:si>
+  <x:si>
+    <x:t>velocity_param</x:t>
+  </x:si>
+  <x:si>
     <x:t>그냥 그때그때 그리는 걸로</x:t>
   </x:si>
   <x:si>
-    <x:t>Ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Na</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pt</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Li</x:t>
-  </x:si>
-  <x:si>
-    <x:t>K</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>velocity_real</x:t>
-  </x:si>
-  <x:si>
-    <x:t>velocity_param</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c(light velocity)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m(electrons' mass)</x:t>
+    <x:t>v : Math.sqrt( 2 * (h * freq - phi - volt) / m),</x:t>
+  </x:si>
+  <x:si>
+    <x:t>문턱진동수[Hz]</x:t>
   </x:si>
   <x:si>
     <x:t>문턱진동수로 두자</x:t>
   </x:si>
   <x:si>
+    <x:t>Intensity</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Retarding V</x:t>
+  </x:si>
+  <x:si>
     <x:t>Frequency</x:t>
   </x:si>
   <x:si>
-    <x:t>Intensity</x:t>
-  </x:si>
-  <x:si>
-    <x:t>문턱진동수[Hz]</x:t>
-  </x:si>
-  <x:si>
     <x:t>Constants</x:t>
   </x:si>
   <x:si>
+    <x:t>h(Planck)</x:t>
+  </x:si>
+  <x:si>
     <x:t>light const</x:t>
   </x:si>
   <x:si>
-    <x:t>h(Planck)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Retarding V</x:t>
+    <x:t>x_val</x:t>
   </x:si>
   <x:si>
     <x:t>Unit</x:t>
   </x:si>
   <x:si>
+    <x:t>y_val</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Value</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cu,Ag</x:t>
+  </x:si>
+  <x:si>
+    <x:t>일함수[eV]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[eV·s]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>eV-Hz</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Metal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>파장[nm]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[kg]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Graph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Freq</x:t>
+  </x:si>
+  <x:si>
     <x:t>[m/s]</x:t>
   </x:si>
   <x:si>
     <x:t>파장[m]</x:t>
   </x:si>
   <x:si>
-    <x:t>파장[nm]</x:t>
+    <x:t>주어진 일함수</x:t>
   </x:si>
   <x:si>
     <x:t>ν const</x:t>
@@ -92,49 +134,7 @@
     <x:t>const</x:t>
   </x:si>
   <x:si>
-    <x:t>주어진 일함수</x:t>
-  </x:si>
-  <x:si>
     <x:t>Default</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[eV·s]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>x_val</x:t>
-  </x:si>
-  <x:si>
-    <x:t>y_val</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Graph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Value</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cu,Ag</x:t>
-  </x:si>
-  <x:si>
-    <x:t>일함수[eV]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>eV-Hz</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Metal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>v : Math.sqrt( 2 * (h * freq - phi - volt) / m),</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[kg]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Freq</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -370,6 +370,35 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
@@ -379,35 +408,6 @@
       </mc:Choice>
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <x:xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -440,6 +440,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -522,6 +523,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -556,6 +558,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -600,6 +603,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -643,6 +647,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -703,6 +708,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -723,6 +729,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -753,6 +760,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -805,7 +813,7 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing0.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1106,7 +1114,7 @@
   <x:dimension ref="B1:O19"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" workbookViewId="0">
-      <x:selection activeCell="Q10" activeCellId="0" sqref="Q10:Q10"/>
+      <x:selection activeCell="Q14" activeCellId="0" sqref="Q14:Q14"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.399999999999999"/>
@@ -1130,30 +1138,30 @@
   <x:sheetData>
     <x:row r="1" spans="12:12">
       <x:c r="L1" s="1" t="s">
-        <x:v>37</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="2:15" customHeight="1">
-      <x:c r="B2" s="11" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C2" s="11"/>
-      <x:c r="D2" s="11"/>
+      <x:c r="B2" s="14" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C2" s="14"/>
+      <x:c r="D2" s="14"/>
       <x:c r="E2" s="2"/>
       <x:c r="F2" s="7" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G2" s="7" t="s">
-        <x:v>34</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H2" s="7" t="s">
-        <x:v>14</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="I2" s="8" t="s">
-        <x:v>21</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="J2" s="8" t="s">
-        <x:v>22</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L2"/>
       <x:c r="M2"/>
@@ -1162,16 +1170,16 @@
     </x:row>
     <x:row r="3" spans="2:15">
       <x:c r="B3" s="6" t="s">
-        <x:v>32</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C3" s="6" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="D3" s="14" t="s">
-        <x:v>19</x:v>
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D3" s="12" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F3" s="5" t="s">
-        <x:v>6</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="G3" s="2">
         <x:v>1.8999999999999999</x:v>
@@ -1187,8 +1195,8 @@
         <x:f>I3*(1000000000)</x:f>
         <x:v>653</x:v>
       </x:c>
-      <x:c r="L3" s="13" t="s">
-        <x:v>39</x:v>
+      <x:c r="L3" s="11" t="s">
+        <x:v>33</x:v>
       </x:c>
       <x:c r="M3" s="1">
         <x:v>10</x:v>
@@ -1204,17 +1212,17 @@
     </x:row>
     <x:row r="4" spans="2:13">
       <x:c r="B4" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C4" s="1">
         <x:f>0.000000000000004136</x:f>
         <x:v>4.1360000000000002E-15</x:v>
       </x:c>
-      <x:c r="D4" s="15" t="s">
+      <x:c r="D4" s="13" t="s">
         <x:v>27</x:v>
       </x:c>
       <x:c r="F4" s="5" t="s">
-        <x:v>5</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G4" s="2">
         <x:v>2.2000000000000002</x:v>
@@ -1230,8 +1238,8 @@
         <x:f>I4*(1000000000)</x:f>
         <x:v>564</x:v>
       </x:c>
-      <x:c r="L4" s="13" t="s">
-        <x:v>7</x:v>
+      <x:c r="L4" s="11" t="s">
+        <x:v>8</x:v>
       </x:c>
       <x:c r="M4" s="1">
         <x:f>SQRT(2*(C4*O3-G3-0)/C6)</x:f>
@@ -1240,13 +1248,13 @@
     </x:row>
     <x:row r="5" spans="2:13">
       <x:c r="B5" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C5" s="3">
         <x:v>299800000</x:v>
       </x:c>
-      <x:c r="D5" s="15" t="s">
-        <x:v>20</x:v>
+      <x:c r="D5" s="13" t="s">
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F5" s="5" t="s">
         <x:v>2</x:v>
@@ -1265,8 +1273,8 @@
         <x:f>I5*(1000000000)</x:f>
         <x:v>539</x:v>
       </x:c>
-      <x:c r="L5" s="13" t="s">
-        <x:v>8</x:v>
+      <x:c r="L5" s="11" t="s">
+        <x:v>9</x:v>
       </x:c>
       <x:c r="M5" s="1">
         <x:f>M4/(1000000000000000)</x:f>
@@ -1275,17 +1283,17 @@
     </x:row>
     <x:row r="6" spans="2:10">
       <x:c r="B6" s="1" t="s">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C6" s="1">
         <x:f>9.1E-31</x:f>
         <x:v>9.1000000000000001E-31</x:v>
       </x:c>
-      <x:c r="D6" s="15" t="s">
-        <x:v>38</x:v>
+      <x:c r="D6" s="13" t="s">
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F6" s="5" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G6" s="2">
         <x:v>2.5</x:v>
@@ -1303,9 +1311,9 @@
       </x:c>
     </x:row>
     <x:row r="7" spans="4:10">
-      <x:c r="D7" s="15"/>
+      <x:c r="D7" s="13"/>
       <x:c r="F7" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="G7" s="2">
         <x:v>3.2000000000000002</x:v>
@@ -1323,9 +1331,9 @@
       </x:c>
     </x:row>
     <x:row r="8" spans="4:10">
-      <x:c r="D8" s="15"/>
+      <x:c r="D8" s="13"/>
       <x:c r="F8" s="5" t="s">
-        <x:v>33</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G8" s="2">
         <x:v>4.7000000000000002</x:v>
@@ -1343,7 +1351,7 @@
       </x:c>
     </x:row>
     <x:row r="9" spans="4:10">
-      <x:c r="D9" s="15"/>
+      <x:c r="D9" s="13"/>
       <x:c r="F9" s="5" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -1363,85 +1371,89 @@
       </x:c>
     </x:row>
     <x:row r="10" spans="4:4">
-      <x:c r="D10" s="15"/>
+      <x:c r="D10" s="13"/>
     </x:row>
     <x:row r="11" spans="6:10" customHeight="1">
-      <x:c r="F11" s="11" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="G11" s="11"/>
-      <x:c r="H11" s="11"/>
-      <x:c r="I11" s="11"/>
-      <x:c r="J11" s="11"/>
+      <x:c r="F11" s="14" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="G11" s="14"/>
+      <x:c r="H11" s="14"/>
+      <x:c r="I11" s="14"/>
+      <x:c r="J11" s="14"/>
     </x:row>
     <x:row r="12" spans="6:10" customHeight="1">
       <x:c r="F12" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G12" s="12" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="H12" s="12"/>
-      <x:c r="I12" s="12"/>
-      <x:c r="J12" s="12"/>
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G12" s="15" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H12" s="15"/>
+      <x:c r="I12" s="15"/>
+      <x:c r="J12" s="15"/>
     </x:row>
     <x:row r="13" spans="6:10" customHeight="1">
       <x:c r="F13" s="5" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G13" s="12"/>
-      <x:c r="H13" s="12"/>
-      <x:c r="I13" s="12"/>
-      <x:c r="J13" s="12"/>
-    </x:row>
-    <x:row r="14" spans="6:10" customHeight="1">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G13" s="15"/>
+      <x:c r="H13" s="15"/>
+      <x:c r="I13" s="15"/>
+      <x:c r="J13" s="15"/>
+    </x:row>
+    <x:row r="14" spans="6:13" customHeight="1">
       <x:c r="F14" s="5" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="G14" s="12">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G14" s="15">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="H14" s="12"/>
-      <x:c r="I14" s="12"/>
-      <x:c r="J14" s="12"/>
+      <x:c r="H14" s="15"/>
+      <x:c r="I14" s="15"/>
+      <x:c r="J14" s="15"/>
+      <x:c r="M14" s="1">
+        <x:f>C4*1*(1000000000000000)-G3</x:f>
+        <x:v>2.2360000000000002</x:v>
+      </x:c>
     </x:row>
     <x:row r="16" spans="6:9">
       <x:c r="F16" s="9" t="s">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G16" s="9" t="s">
-        <x:v>28</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H16" s="9" t="s">
-        <x:v>29</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="I16" s="9" t="s">
-        <x:v>24</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="6:10" customHeight="1">
       <x:c r="F17" s="10" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="G17" s="12" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="H17" s="12"/>
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="G17" s="15" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H17" s="15"/>
       <x:c r="I17" s="10"/>
       <x:c r="J17" s="10"/>
     </x:row>
     <x:row r="18" spans="6:9">
       <x:c r="F18" s="10" t="s">
-        <x:v>23</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G18" s="1"/>
       <x:c r="I18" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="6:9">
       <x:c r="F19" s="10" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="G19" s="1"/>
       <x:c r="I19" s="10">
@@ -1457,7 +1469,7 @@
     <x:mergeCell ref="G14:J14"/>
     <x:mergeCell ref="G17:H17"/>
   </x:mergeCells>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51152777671813965" footer="0.51152777671813965"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51138889789581299" footer="0.51138889789581299"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <x:drawing r:id="rId1"/>
 </x:worksheet>
@@ -1474,7 +1486,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.35"/>
   <x:sheetData/>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51152777671813965" footer="0.51152777671813965"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51138889789581299" footer="0.51138889789581299"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -1490,7 +1502,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.35"/>
   <x:sheetData/>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51152777671813965" footer="0.51152777671813965"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51138889789581299" footer="0.51138889789581299"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>